<commit_message>
lots of updates to powerSpectra and lag
Completed powerSpectra pipeline
added functions to plot powermap and powerspectra
renamed function to examplePowerAnalysis
added preliminary pipeline for lag analysis on Asher's data
copied over Kenny's parser functions
</commit_message>
<xml_diff>
--- a/excelFile.xlsx
+++ b/excelFile.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100662A3-226B-4DF2-B555-4015668C0390}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E582D63-F4FA-4DC1-B273-B7F4EE254522}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -122,6 +123,12 @@
   </si>
   <si>
     <t>C:\Users\Nischal\Documents\MATLAB_Test\TestProcessed</t>
+  </si>
+  <si>
+    <t>D:\ProcessedData\FAD-GcAMP-New</t>
+  </si>
+  <si>
+    <t>Sampling Rate Fluor</t>
   </si>
 </sst>
 </file>
@@ -171,7 +178,70 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="54">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -763,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,9 +850,10 @@
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -810,8 +881,11 @@
       <c r="I1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>181031</v>
       </c>
@@ -837,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>190530</v>
       </c>
@@ -866,7 +940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>190530</v>
       </c>
@@ -895,7 +969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>190530</v>
       </c>
@@ -924,7 +998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>190530</v>
       </c>
@@ -953,7 +1027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>190527</v>
       </c>
@@ -982,7 +1056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>190527</v>
       </c>
@@ -1011,7 +1085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>190527</v>
       </c>
@@ -1040,7 +1114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>190527</v>
       </c>
@@ -1069,7 +1143,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>190527</v>
       </c>
@@ -1098,7 +1172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>190527</v>
       </c>
@@ -1127,7 +1201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>190527</v>
       </c>
@@ -1156,7 +1230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>190527</v>
       </c>
@@ -1185,7 +1259,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>180917</v>
       </c>
@@ -1214,7 +1288,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>180917</v>
       </c>
@@ -1243,7 +1317,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>180917</v>
       </c>
@@ -1272,7 +1346,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>180917</v>
       </c>
@@ -1301,7 +1375,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>180917</v>
       </c>
@@ -1330,7 +1404,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>180917</v>
       </c>
@@ -1359,223 +1433,369 @@
         <v>16.8</v>
       </c>
     </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>190530</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>9</v>
+      </c>
+      <c r="J21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>190530</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+      <c r="I22">
+        <v>9</v>
+      </c>
+      <c r="J22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>190530</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B2 D2:F2 A1:G1">
-    <cfRule type="expression" dxfId="44" priority="57">
+    <cfRule type="expression" dxfId="53" priority="67">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
+    <cfRule type="expression" dxfId="52" priority="56">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="expression" dxfId="51" priority="55">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="expression" dxfId="50" priority="54">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="expression" dxfId="49" priority="53">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="expression" dxfId="48" priority="52">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="expression" dxfId="47" priority="51">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="expression" dxfId="46" priority="50">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="expression" dxfId="45" priority="49">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="expression" dxfId="44" priority="48">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="expression" dxfId="43" priority="47">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
     <cfRule type="expression" dxfId="42" priority="46">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
+  <conditionalFormatting sqref="E7">
     <cfRule type="expression" dxfId="41" priority="45">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
+  <conditionalFormatting sqref="F7">
     <cfRule type="expression" dxfId="40" priority="44">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
+  <conditionalFormatting sqref="D8">
     <cfRule type="expression" dxfId="39" priority="43">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
+  <conditionalFormatting sqref="E8">
     <cfRule type="expression" dxfId="38" priority="42">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
+  <conditionalFormatting sqref="F8">
     <cfRule type="expression" dxfId="37" priority="41">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
+  <conditionalFormatting sqref="D9">
     <cfRule type="expression" dxfId="36" priority="40">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
+  <conditionalFormatting sqref="E9">
     <cfRule type="expression" dxfId="35" priority="39">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
+  <conditionalFormatting sqref="F9">
     <cfRule type="expression" dxfId="34" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
+  <conditionalFormatting sqref="D10">
     <cfRule type="expression" dxfId="33" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
+  <conditionalFormatting sqref="E10">
     <cfRule type="expression" dxfId="32" priority="36">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
+  <conditionalFormatting sqref="F10">
     <cfRule type="expression" dxfId="31" priority="35">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7">
+  <conditionalFormatting sqref="D11">
     <cfRule type="expression" dxfId="30" priority="34">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+  <conditionalFormatting sqref="E11">
     <cfRule type="expression" dxfId="29" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+  <conditionalFormatting sqref="F11">
     <cfRule type="expression" dxfId="28" priority="32">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
+  <conditionalFormatting sqref="D12">
     <cfRule type="expression" dxfId="27" priority="31">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
+  <conditionalFormatting sqref="E12">
     <cfRule type="expression" dxfId="26" priority="30">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="25" priority="29">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
+  <conditionalFormatting sqref="D13">
     <cfRule type="expression" dxfId="24" priority="28">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
+  <conditionalFormatting sqref="E13">
     <cfRule type="expression" dxfId="23" priority="27">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="F13">
     <cfRule type="expression" dxfId="22" priority="26">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
+  <conditionalFormatting sqref="D14">
     <cfRule type="expression" dxfId="21" priority="25">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
+  <conditionalFormatting sqref="E14">
     <cfRule type="expression" dxfId="20" priority="24">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
+  <conditionalFormatting sqref="F14">
     <cfRule type="expression" dxfId="19" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="I1">
     <cfRule type="expression" dxfId="18" priority="22">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
+  <conditionalFormatting sqref="F15">
     <cfRule type="expression" dxfId="17" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="16" priority="20">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="15" priority="19">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="14" priority="18">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="13" priority="17">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="11" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="10" priority="14">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="9" priority="13">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1">
-    <cfRule type="expression" dxfId="8" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15">
-    <cfRule type="expression" dxfId="7" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="16" priority="19">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="15" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
updating with more code
</commit_message>
<xml_diff>
--- a/excelFile.xlsx
+++ b/excelFile.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F2B664-466A-4962-8DE9-510EB05A54B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88A1B82-307A-4D55-B1A5-913C7C9B3CA0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="960" windowWidth="19920" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -214,10 +214,13 @@
     <t>G11M2-awake</t>
   </si>
   <si>
-    <t>F:\fromXiaodan\Processed</t>
-  </si>
-  <si>
-    <t>F:\fromXiaodan</t>
+    <t>G26M4</t>
+  </si>
+  <si>
+    <t>D:\ProcessedData\TestData</t>
+  </si>
+  <si>
+    <t>C:\Users\Nischal\Documents\QuickTestData</t>
   </si>
 </sst>
 </file>
@@ -461,17 +464,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
-    <dxf>
-      <font>
-        <color rgb="FF124E13"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFBC0000"/>
-      </font>
-    </dxf>
+  <dxfs count="72">
     <dxf>
       <font>
         <color rgb="FF124E13"/>
@@ -1118,13 +1111,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C62" sqref="C62"/>
+      <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3076,10 +3069,10 @@
         <v>61</v>
       </c>
       <c r="C59" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D59" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="E59" s="10" t="s">
         <v>4</v>
@@ -3103,292 +3096,327 @@
         <v>1</v>
       </c>
     </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>190905</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="12">
+        <v>20</v>
+      </c>
+      <c r="H60" s="4">
+        <v>100</v>
+      </c>
+      <c r="I60" s="12">
+        <v>9</v>
+      </c>
+      <c r="J60" s="20">
+        <v>9</v>
+      </c>
+      <c r="K60" s="23">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F21 F37 F49 F59:F1048576">
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="71" priority="74" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="70" priority="73" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="containsText" dxfId="71" priority="71" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="69" priority="71" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="72" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="68" priority="72" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="67" priority="69" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="70" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="66" priority="70" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="containsText" dxfId="67" priority="67" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="68" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="containsText" dxfId="65" priority="63" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="63" priority="63" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="64" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="62" priority="64" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="containsText" dxfId="63" priority="61" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="61" priority="61" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="62" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="60" priority="62" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="containsText" dxfId="61" priority="59" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="59" priority="59" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="60" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="58" priority="60" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="containsText" dxfId="59" priority="57" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="57" priority="57" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="58" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="56" priority="58" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="55" priority="55" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="54" priority="56" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="53" priority="53" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="52" priority="54" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="containsText" dxfId="53" priority="51" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="52" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="50" priority="52" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="containsText" dxfId="51" priority="49" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="49" priority="49" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="50" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="48" priority="50" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F33">
-    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="47" priority="47" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="46" priority="48" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="containsText" dxfId="45" priority="43" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="43" priority="43" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="44" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="42" priority="44" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36">
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38">
-    <cfRule type="containsText" dxfId="41" priority="39" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="40" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39">
-    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="37" priority="37" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="36" priority="38" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40">
-    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43">
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44">
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45">
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46">
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47">
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F53">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="fc">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F58)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
cleanup and restructure of code and folders
</commit_message>
<xml_diff>
--- a/excelFile.xlsx
+++ b/excelFile.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88A1B82-307A-4D55-B1A5-913C7C9B3CA0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85957857-47FC-419D-9EB5-983A2A250636}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -257,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,6 +315,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -460,11 +466,41 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="76">
+    <dxf>
+      <font>
+        <color rgb="FF124E13"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFBC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF124E13"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFBC0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF124E13"/>
@@ -1111,13 +1147,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
+      <selection pane="bottomRight" activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3131,293 +3167,414 @@
         <v>1</v>
       </c>
     </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="46">
+        <v>181116</v>
+      </c>
+      <c r="B61" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D61" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G61" s="43">
+        <v>16.8</v>
+      </c>
+      <c r="H61" s="43">
+        <v>0</v>
+      </c>
+      <c r="I61" s="43">
+        <v>16.8</v>
+      </c>
+      <c r="J61" s="44">
+        <v>16.8</v>
+      </c>
+      <c r="K61" s="45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="46">
+        <v>181116</v>
+      </c>
+      <c r="B62" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G62" s="43">
+        <v>16.8</v>
+      </c>
+      <c r="H62" s="43">
+        <v>0</v>
+      </c>
+      <c r="I62" s="43">
+        <v>16.8</v>
+      </c>
+      <c r="J62" s="44">
+        <v>16.8</v>
+      </c>
+      <c r="K62" s="45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="46">
+        <v>181116</v>
+      </c>
+      <c r="B63" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D63" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F63" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G63" s="43">
+        <v>16.8</v>
+      </c>
+      <c r="H63" s="43">
+        <v>0</v>
+      </c>
+      <c r="I63" s="43">
+        <v>16.8</v>
+      </c>
+      <c r="J63" s="44">
+        <v>16.8</v>
+      </c>
+      <c r="K63" s="45">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F21 F37 F49 F59:F1048576">
-    <cfRule type="containsText" dxfId="71" priority="74" operator="containsText" text="fc">
+  <conditionalFormatting sqref="F1:F21 F37 F49 F59:F61 F64:F1048576">
+    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="73" operator="containsText" text="stim">
+    <cfRule type="containsText" dxfId="74" priority="77" operator="containsText" text="stim">
       <formula>NOT(ISERROR(SEARCH("stim",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
+    <cfRule type="containsText" dxfId="73" priority="75" operator="containsText" text="stim">
+      <formula>NOT(ISERROR(SEARCH("stim",F22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="76" operator="containsText" text="fc">
+      <formula>NOT(ISERROR(SEARCH("fc",F22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="containsText" dxfId="71" priority="73" operator="containsText" text="stim">
+      <formula>NOT(ISERROR(SEARCH("stim",F23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="74" operator="containsText" text="fc">
+      <formula>NOT(ISERROR(SEARCH("fc",F23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
     <cfRule type="containsText" dxfId="69" priority="71" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F24)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="68" priority="72" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F23">
-    <cfRule type="containsText" dxfId="67" priority="69" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="70" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F24">
-    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="fc">
       <formula>NOT(ISERROR(SEARCH("fc",F24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
+    <cfRule type="containsText" dxfId="67" priority="67" operator="containsText" text="stim">
+      <formula>NOT(ISERROR(SEARCH("stim",F25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="68" operator="containsText" text="fc">
+      <formula>NOT(ISERROR(SEARCH("fc",F25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="containsText" dxfId="65" priority="65" operator="containsText" text="stim">
+      <formula>NOT(ISERROR(SEARCH("stim",F26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="66" operator="containsText" text="fc">
+      <formula>NOT(ISERROR(SEARCH("fc",F26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
     <cfRule type="containsText" dxfId="63" priority="63" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F25)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F27)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="62" priority="64" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26">
+      <formula>NOT(ISERROR(SEARCH("fc",F27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
     <cfRule type="containsText" dxfId="61" priority="61" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F26)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F28)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="60" priority="62" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
+      <formula>NOT(ISERROR(SEARCH("fc",F28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29">
     <cfRule type="containsText" dxfId="59" priority="59" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F29)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="58" priority="60" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
+      <formula>NOT(ISERROR(SEARCH("fc",F29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30">
     <cfRule type="containsText" dxfId="57" priority="57" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F28)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F30)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="56" priority="58" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
+      <formula>NOT(ISERROR(SEARCH("fc",F30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F31">
     <cfRule type="containsText" dxfId="55" priority="55" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F29)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F31)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="54" priority="56" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30">
+      <formula>NOT(ISERROR(SEARCH("fc",F31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32">
     <cfRule type="containsText" dxfId="53" priority="53" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F30)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F32)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="52" priority="54" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F31">
+      <formula>NOT(ISERROR(SEARCH("fc",F32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F33">
     <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F31)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="50" priority="52" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F32">
+      <formula>NOT(ISERROR(SEARCH("fc",F33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F34">
     <cfRule type="containsText" dxfId="49" priority="49" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F32)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="48" priority="50" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F33">
+      <formula>NOT(ISERROR(SEARCH("fc",F34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35">
     <cfRule type="containsText" dxfId="47" priority="47" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F35)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="46" priority="48" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F34">
+      <formula>NOT(ISERROR(SEARCH("fc",F35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36">
     <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F34)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F36)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
+      <formula>NOT(ISERROR(SEARCH("fc",F36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F38">
     <cfRule type="containsText" dxfId="43" priority="43" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F38)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="42" priority="44" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F36">
+      <formula>NOT(ISERROR(SEARCH("fc",F38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
     <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F36)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F39)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F38">
+      <formula>NOT(ISERROR(SEARCH("fc",F39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40">
     <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
+      <formula>NOT(ISERROR(SEARCH("fc",F40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41">
     <cfRule type="containsText" dxfId="37" priority="37" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F39)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F41)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="36" priority="38" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
+      <formula>NOT(ISERROR(SEARCH("fc",F41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42">
     <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F40)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F42)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F41">
+      <formula>NOT(ISERROR(SEARCH("fc",F42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43">
     <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F43)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F42">
+      <formula>NOT(ISERROR(SEARCH("fc",F43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44">
     <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F44)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
+      <formula>NOT(ISERROR(SEARCH("fc",F44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45">
     <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F43)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F45)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44">
+      <formula>NOT(ISERROR(SEARCH("fc",F45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46">
     <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F44)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F46)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
+      <formula>NOT(ISERROR(SEARCH("fc",F46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47">
     <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F45)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F47)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46">
+      <formula>NOT(ISERROR(SEARCH("fc",F47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F48)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
+      <formula>NOT(ISERROR(SEARCH("fc",F48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50">
     <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F47)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F50)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48">
+      <formula>NOT(ISERROR(SEARCH("fc",F50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F51">
     <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F51)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F50">
+      <formula>NOT(ISERROR(SEARCH("fc",F51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F52">
     <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F50)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F52)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F50)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F51">
+      <formula>NOT(ISERROR(SEARCH("fc",F52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F53">
     <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F51)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F53)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F52">
+      <formula>NOT(ISERROR(SEARCH("fc",F53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F54">
     <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F52)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F52)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F53">
+      <formula>NOT(ISERROR(SEARCH("fc",F54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F55">
     <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F55)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F54">
+      <formula>NOT(ISERROR(SEARCH("fc",F55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F56">
     <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F56)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F55">
+      <formula>NOT(ISERROR(SEARCH("fc",F56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F57">
     <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F57)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F56">
+      <formula>NOT(ISERROR(SEARCH("fc",F57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F58">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F56)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F57">
+      <formula>NOT(ISERROR(SEARCH("fc",F58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F62">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F58">
+      <formula>NOT(ISERROR(SEARCH("fc",F62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F63">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="stim">
-      <formula>NOT(ISERROR(SEARCH("stim",F58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("stim",F63)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="fc">
-      <formula>NOT(ISERROR(SEARCH("fc",F58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("fc",F63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>